<commit_message>
W.I.P. check-in. 'Madden 18 Player Ratings.csv' should now be final; do one more run with all teams to make sure. Working on the function for finding a player's contract page on OTC.com - plan to merge the two loops into one, after whichever name match method worked,
</commit_message>
<xml_diff>
--- a/docs/Player Fields and Values.xlsx
+++ b/docs/Player Fields and Values.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Updater - WORKING COPY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Gaming\madden_08_updater\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -4151,7 +4151,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4695,8 +4695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F768"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A516" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F516" sqref="F516"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
WIP - Working on helper methods for creating players. So far, so good. Have most direct-from-CSV fields, names, teams, and a college placeholder.
</commit_message>
<xml_diff>
--- a/docs/Player Fields and Values.xlsx
+++ b/docs/Player Fields and Values.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="1375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1873" uniqueCount="1376">
   <si>
     <t>Field</t>
   </si>
@@ -4146,6 +4146,9 @@
   </si>
   <si>
     <t>Vast majority have 0. No difference seen in the player editor, or noticed in-game.</t>
+  </si>
+  <si>
+    <t>SIGNED Int; -49 - 49</t>
   </si>
 </sst>
 </file>
@@ -4729,7 +4732,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F768"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A215" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D239" sqref="D239"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11945,7 +11950,9 @@
       <c r="D696" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="E696" s="22"/>
+      <c r="E696" s="22" t="s">
+        <v>1029</v>
+      </c>
       <c r="F696" s="23" t="s">
         <v>1255</v>
       </c>
@@ -11963,7 +11970,9 @@
       <c r="D697" s="26" t="s">
         <v>1257</v>
       </c>
-      <c r="E697" s="26"/>
+      <c r="E697" s="26" t="s">
+        <v>1025</v>
+      </c>
       <c r="F697" s="27" t="s">
         <v>1258</v>
       </c>
@@ -11981,7 +11990,9 @@
       <c r="D698" s="22" t="s">
         <v>1260</v>
       </c>
-      <c r="E698" s="22"/>
+      <c r="E698" s="22" t="s">
+        <v>1025</v>
+      </c>
       <c r="F698" s="23" t="s">
         <v>1259</v>
       </c>
@@ -11999,7 +12010,9 @@
       <c r="D699" s="26" t="s">
         <v>1264</v>
       </c>
-      <c r="E699" s="26"/>
+      <c r="E699" s="26" t="s">
+        <v>1025</v>
+      </c>
       <c r="F699" s="27" t="s">
         <v>1262</v>
       </c>
@@ -12017,7 +12030,9 @@
       <c r="D700" s="22" t="s">
         <v>1265</v>
       </c>
-      <c r="E700" s="22"/>
+      <c r="E700" s="22" t="s">
+        <v>1025</v>
+      </c>
       <c r="F700" s="23" t="s">
         <v>1266</v>
       </c>
@@ -12035,7 +12050,9 @@
       <c r="D701" s="26" t="s">
         <v>1257</v>
       </c>
-      <c r="E701" s="26"/>
+      <c r="E701" s="26" t="s">
+        <v>1025</v>
+      </c>
       <c r="F701" s="27" t="s">
         <v>1268</v>
       </c>
@@ -12053,7 +12070,9 @@
       <c r="D702" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E702" s="14"/>
+      <c r="E702" s="14" t="s">
+        <v>1032</v>
+      </c>
       <c r="F702" s="15" t="s">
         <v>1270</v>
       </c>
@@ -12148,7 +12167,9 @@
       <c r="D710" s="26" t="s">
         <v>1279</v>
       </c>
-      <c r="E710" s="26"/>
+      <c r="E710" s="26" t="s">
+        <v>1032</v>
+      </c>
     </row>
     <row r="711" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A711" s="11" t="s">
@@ -12163,7 +12184,9 @@
       <c r="D711" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E711" s="10"/>
+      <c r="E711" s="10" t="s">
+        <v>1032</v>
+      </c>
       <c r="F711" s="11" t="s">
         <v>1270</v>
       </c>
@@ -12258,7 +12281,9 @@
       <c r="D719" s="26" t="s">
         <v>1279</v>
       </c>
-      <c r="E719" s="26"/>
+      <c r="E719" s="26" t="s">
+        <v>1032</v>
+      </c>
     </row>
     <row r="720" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A720" s="23" t="s">
@@ -12887,7 +12912,9 @@
       <c r="D765" s="52" t="s">
         <v>1320</v>
       </c>
-      <c r="E765" s="52"/>
+      <c r="E765" s="52" t="s">
+        <v>1375</v>
+      </c>
       <c r="F765" s="31" t="s">
         <v>1321</v>
       </c>

</xml_diff>

<commit_message>
Finished player-specific final steps for: QB, HB, FB, WR, TE, LT. Filled out 'player_roles' further to support player-specific code. Updated TODO list. Updated 'Methods...' to mark completed work as completed.
</commit_message>
<xml_diff>
--- a/docs/Player Fields and Values.xlsx
+++ b/docs/Player Fields and Values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Gaming\madden_08_updater\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD9C1AF-EE8C-4CCB-91C2-7389F1431509}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EEC734-7D4B-44A5-B860-1F5E66E22B3F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="915" windowWidth="9240" windowHeight="3060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2390" uniqueCount="1620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2390" uniqueCount="1621">
   <si>
     <t>Field</t>
   </si>
@@ -4882,6 +4882,9 @@
   </si>
   <si>
     <t>FEATURE BACK: (Just indicates exceptional SPD + ACC + AGI? No requirements, benefits named.) POS = HB only</t>
+  </si>
+  <si>
+    <t>TEAM MENTOR: Value +5%. Removed if player's OVR &lt; 86 and MOR &lt; 26 at end of season. Gives young position mates AWR +2, older ones AWR +1.</t>
   </si>
 </sst>
 </file>
@@ -5465,8 +5468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A511" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F527" sqref="F527"/>
+    <sheetView tabSelected="1" topLeftCell="A505" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F532" sqref="F532"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10613,7 +10616,7 @@
       </c>
       <c r="E521" s="14"/>
       <c r="F521" s="15" t="s">
-        <v>1230</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="522" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
More player-specific final code for: LT, LG, C, RG, RT, LE, RE, DT. Related player_roles and 'Methods...' updates and additions.
</commit_message>
<xml_diff>
--- a/docs/Player Fields and Values.xlsx
+++ b/docs/Player Fields and Values.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Gaming\madden_08_updater\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EEC734-7D4B-44A5-B860-1F5E66E22B3F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2326C600-64BE-4860-8DF9-B1F08A7BEFC6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="915" windowWidth="9240" windowHeight="3060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5468,8 +5468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A505" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F532" sqref="F532"/>
+    <sheetView tabSelected="1" topLeftCell="A514" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F544" sqref="F544"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>